<commit_message>
add barcode and getprice
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -855,6 +855,426 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>BK</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>PM</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1234</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>cdf24541-9127-458c-9cd5-b8a12f4b929c</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-03-11T13:53:26.610680</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2025-03-11T13:55:06.282262</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>BK</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>PM</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2345</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>6d8fbad6-85c0-425a-a3dc-61f9817d2009</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-03-11T13:53:30.710633</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2025-03-11T13:53:32.391061</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>BK</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>PM</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1234</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>6bfd6e1c-2f99-4993-94fb-c8f296212a53</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-03-11T13:54:54.693445</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2025-03-11T14:08:24.249050</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>BK</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>PM</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2456</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>27daef15-51da-4a46-a80d-325cc956802e</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-03-11T13:54:59.197709</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2025-03-11T14:08:24.386535</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>BK</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>PM</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1234</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>31388b15-ac05-400d-a303-d5f639f45404</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-03-11T13:55:40.379223</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2025-03-12T11:03:48.781585</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>BK</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>PM</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1245</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>3864c7a9-753a-467e-9e3d-d05048ff16d7</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-03-11T13:55:44.585014</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>2025-03-12T11:03:45.695443</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>BK</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>PM</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>5678</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>e2b508a8-f1a7-42e2-a070-a2f670779e15</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-03-11T13:55:47.751952</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2025-03-11T14:09:28.875654</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>BK</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>PM</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1234</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>1693ac31-331b-4156-90d9-98c1b862bfdc</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-03-11T13:59:02.371825</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2025-03-12T11:03:47.019402</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>BK</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>PM</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1234</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>c6559d3d-b592-4d32-b93a-d6f4ebaf2da4</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-03-12T08:09:09.694421</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>2025-03-12T11:03:47.790109</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>BK</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>PM</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1233</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>cbf07666-709f-480c-ac5c-0b2b784cc3b9</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-03-12T08:09:13.875922</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2025-03-12T11:03:49.283978</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>BK</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>PM</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>3456</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>fa885632-045e-48ce-bca3-39f8a6d56b28</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-03-12T08:25:51.334453</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2025-03-12T09:42:06.423077</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>BK</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>PM</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>1234</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>9106c101-5720-4d4a-a8d0-337c6d325549</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-03-12T08:27:38.952059</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2025-03-12T08:27:40.743786</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>